<commit_message>
re-running hotspots controllong for effort for sponge % cover estimates
</commit_message>
<xml_diff>
--- a/Data/logistic regression results.xlsx
+++ b/Data/logistic regression results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylel\OneDrive\Documents\GitHub\ccira-rockfish\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A3CDB4-730C-41A6-B392-56FE57101504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937A0C45-B783-4696-BF4E-5A2E0492FF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D938339-D3ED-4BF4-83E1-ADA1B8713C40}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <r>
       <t>Table 3</t>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -286,9 +286,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -298,10 +295,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -618,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A42912-B20A-455D-9970-1C3403DABD2F}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,234 +649,253 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>3.6</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>2.72</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1.32</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>-5.88</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2.71</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>-2.17</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>-0.13</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.89</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.59</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.22</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>2.71</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>0.01</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>22.07</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>2.86</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>7.73</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>1.1E-14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>-11.31</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>2.7450000000000001</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>-4.12</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>2.8E-5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>-0.61</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>0.47</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>-1.29</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6">
-        <v>-6.3099999999999996E-3</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2.2899999999999999E-3</v>
-      </c>
-      <c r="E10" s="5">
-        <v>-2.75</v>
+      <c r="C10" s="5">
+        <v>-49.85</v>
+      </c>
+      <c r="D10" s="5">
+        <v>23.08</v>
+      </c>
+      <c r="E10" s="4">
+        <v>-2.16</v>
       </c>
       <c r="F10" s="5">
-        <v>6.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-40.14</v>
+      </c>
+      <c r="D11" s="5">
+        <v>15.64</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-2.57</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5">
-        <v>-2.13</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.44</v>
-      </c>
-      <c r="E11" s="5">
-        <v>-4.8899999999999997</v>
-      </c>
-      <c r="F11" s="6">
-        <v>9.9000000000000005E-7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="C12" s="4">
+        <v>-1.48</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.35</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-4.2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2.6999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="6">
-        <v>2.04</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2.73</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3.15</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.02</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6">
-        <v>-6.61</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2.92</v>
-      </c>
-      <c r="E13" s="5">
-        <v>-2.2599999999999998</v>
-      </c>
-      <c r="F13" s="5">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5">
+        <v>-12.8</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3.24</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-3.95</v>
+      </c>
+      <c r="F14" s="5">
+        <v>7.8999999999999996E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="5">
-        <v>-1.35</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="E14" s="5">
-        <v>-3.83</v>
-      </c>
-      <c r="F14" s="6">
-        <v>1E-4</v>
+      <c r="C15" s="4">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-3.28</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
find the peaks of the logistic regression
</commit_message>
<xml_diff>
--- a/Data/logistic regression results.xlsx
+++ b/Data/logistic regression results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylel\OneDrive\Documents\GitHub\ccira-rockfish\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937A0C45-B783-4696-BF4E-5A2E0492FF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8873B4-E04D-4485-9103-7EBC3167DD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D938339-D3ED-4BF4-83E1-ADA1B8713C40}"/>
   </bookViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A42912-B20A-455D-9970-1C3403DABD2F}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,16 +656,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="5">
-        <v>3.6</v>
+        <v>1.03E-2</v>
       </c>
       <c r="D3" s="5">
-        <v>2.72</v>
+        <v>3.8300000000000001E-3</v>
       </c>
       <c r="E3" s="4">
-        <v>1.32</v>
+        <v>2.68</v>
       </c>
       <c r="F3" s="4">
-        <v>0.19</v>
+        <v>7.3000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -674,10 +674,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="5">
-        <v>-5.88</v>
+        <v>-2.1500000000000001E-5</v>
       </c>
       <c r="D4" s="5">
-        <v>2.71</v>
+        <v>9.91E-6</v>
       </c>
       <c r="E4" s="4">
         <v>-2.17</v>
@@ -691,8 +691,8 @@
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4">
-        <v>-7.0000000000000007E-2</v>
+      <c r="C5" s="5">
+        <v>-7.3800000000000004E-2</v>
       </c>
       <c r="D5" s="4">
         <v>0.56000000000000005</v>
@@ -709,17 +709,17 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.59</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.22</v>
+      <c r="C6" s="5">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.217</v>
       </c>
       <c r="E6" s="4">
         <v>2.71</v>
       </c>
       <c r="F6" s="5">
-        <v>0.01</v>
+        <v>6.7000000000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -730,16 +730,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="5">
-        <v>22.07</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="D7" s="5">
-        <v>2.86</v>
+        <v>4.7499999999999999E-3</v>
       </c>
       <c r="E7" s="4">
-        <v>7.73</v>
+        <v>5.95</v>
       </c>
       <c r="F7" s="5">
-        <v>1.1E-14</v>
+        <v>2.6000000000000001E-9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -748,16 +748,16 @@
         <v>10</v>
       </c>
       <c r="C8" s="5">
-        <v>-11.31</v>
+        <v>-4.1600000000000002E-5</v>
       </c>
       <c r="D8" s="5">
-        <v>2.7450000000000001</v>
+        <v>1.01E-5</v>
       </c>
       <c r="E8" s="4">
         <v>-4.12</v>
       </c>
       <c r="F8" s="5">
-        <v>2.8E-5</v>
+        <v>3.8000000000000002E-5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -765,11 +765,11 @@
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4">
-        <v>-0.61</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.47</v>
+      <c r="C9" s="5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.47399999999999998</v>
       </c>
       <c r="E9" s="4">
         <v>-1.29</v>
@@ -786,16 +786,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="5">
-        <v>-49.85</v>
+        <v>2.9700000000000001E-2</v>
       </c>
       <c r="D10" s="5">
-        <v>23.08</v>
+        <v>1.03E-2</v>
       </c>
       <c r="E10" s="4">
-        <v>-2.16</v>
+        <v>2.89</v>
       </c>
       <c r="F10" s="5">
-        <v>0.03</v>
+        <v>3.8E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -804,16 +804,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="5">
-        <v>-40.14</v>
+        <v>-1.4799999999999999E-4</v>
       </c>
       <c r="D11" s="5">
-        <v>15.64</v>
+        <v>5.7500000000000002E-5</v>
       </c>
       <c r="E11" s="4">
         <v>-2.57</v>
       </c>
       <c r="F11" s="5">
-        <v>0.01</v>
+        <v>1.03E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -842,16 +842,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="5">
-        <v>3.2</v>
+        <v>0.02</v>
       </c>
       <c r="D13" s="5">
-        <v>3.15</v>
+        <v>4.2700000000000004E-3</v>
       </c>
       <c r="E13" s="4">
-        <v>1.02</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0.31</v>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2.7E-6</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -860,10 +860,10 @@
         <v>10</v>
       </c>
       <c r="C14" s="5">
-        <v>-12.8</v>
+        <v>-4.6999999999999997E-5</v>
       </c>
       <c r="D14" s="5">
-        <v>3.24</v>
+        <v>1.19E-5</v>
       </c>
       <c r="E14" s="4">
         <v>-3.95</v>

</xml_diff>